<commit_message>
graph name caching result
</commit_message>
<xml_diff>
--- a/bsbm/results/results.xlsx
+++ b/bsbm/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minor/projects/twks-benchmarks/bsbm/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5633CBCA-B4F1-0445-B0FA-AD4F770D9061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34720EB0-B800-2641-B40F-71C73DE359FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{3AB62A67-2EB4-D04E-9F3E-A1F2092B6980}"/>
+    <workbookView xWindow="-38740" yWindow="460" windowWidth="38400" windowHeight="19300" xr2:uid="{3AB62A67-2EB4-D04E-9F3E-A1F2092B6980}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Timestamp</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>TDB2 persistent</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Graph name cache enabled</t>
+  </si>
+  <si>
+    <t>~ Halve runtime and double throughput</t>
   </si>
 </sst>
 </file>
@@ -430,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A33573-6F0A-EA48-89CB-E02E0AEAEEDC}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,7 +450,7 @@
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,10 +488,13 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>201911251557</v>
       </c>
@@ -521,6 +533,50 @@
       </c>
       <c r="M2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>201911271207</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>500</v>
+      </c>
+      <c r="G3">
+        <v>0.79339999999999999</v>
+      </c>
+      <c r="H3">
+        <v>2.0379</v>
+      </c>
+      <c r="I3">
+        <v>622.39400000000001</v>
+      </c>
+      <c r="J3">
+        <v>2892.06</v>
+      </c>
+      <c r="K3">
+        <v>1.2447900000000001</v>
+      </c>
+      <c r="L3">
+        <v>1.2295199999999999</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>